<commit_message>
primeira versão da aval360 e att burndown
</commit_message>
<xml_diff>
--- a/SprintLogs/Burndown/burndown_sprint2.xlsx
+++ b/SprintLogs/Burndown/burndown_sprint2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\André\Desktop\DevMinds\SprintLogs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995250A5-FF6C-486C-984E-3B6F8B63336C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169FE357-17AB-4745-A1B5-FB7AA7615CA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{BE849934-861F-4930-8CEE-31DE7D069627}"/>
   </bookViews>
@@ -123,11 +123,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,6 +506,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1618,8 +1621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D0CC0E-94B3-4F4B-B440-BE94AA8B047E}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,17 +1635,17 @@
     <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1656,11 +1659,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>45019</v>
       </c>
       <c r="C3">
@@ -1670,11 +1673,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>45020</v>
       </c>
       <c r="C4">
@@ -1683,133 +1686,138 @@
       <c r="D4">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>45021</v>
       </c>
       <c r="C5">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>45022</v>
       </c>
       <c r="C6">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>45023</v>
       </c>
       <c r="C7">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>45024</v>
       </c>
       <c r="C8">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>45025</v>
       </c>
       <c r="C9">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>45026</v>
       </c>
       <c r="C10">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>45027</v>
       </c>
       <c r="C11">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>45028</v>
       </c>
       <c r="C12">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>45029</v>
       </c>
       <c r="C13">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>45030</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>45031</v>
       </c>
       <c r="C15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>45032</v>
       </c>
       <c r="C16">
@@ -1820,7 +1828,7 @@
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>45033</v>
       </c>
       <c r="C17">
@@ -1831,7 +1839,7 @@
       <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>45034</v>
       </c>
       <c r="C18">
@@ -1842,7 +1850,7 @@
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>45035</v>
       </c>
       <c r="C19">
@@ -1853,7 +1861,7 @@
       <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>45036</v>
       </c>
       <c r="C20">
@@ -1864,7 +1872,7 @@
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>45037</v>
       </c>
       <c r="C21">
@@ -1875,19 +1883,19 @@
       <c r="A22" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>45038</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="J22" s="3"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>45039</v>
       </c>
       <c r="C23">

</xml_diff>